<commit_message>
Categories colours updated to match in every chart
Signed-off-by: Marcos Tavorda <mtavor@hotmail.com>
</commit_message>
<xml_diff>
--- a/Documentación/PLAN 2020-2021/Seguimiento Sprints.xlsx
+++ b/Documentación/PLAN 2020-2021/Seguimiento Sprints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MT\Desktop\Proyecto\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4322D72B-23B7-4AB6-99CE-DD809C05D981}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80911559-E9BA-4D33-A485-547308F45462}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -998,9 +998,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFA94D0F"/>
       <color rgb="FFFF5050"/>
       <color rgb="FF9E5ECE"/>
-      <color rgb="FFA94D0F"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1111,9 +1111,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -1531,7 +1529,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3"/>
+              <a:srgbClr val="FF5050"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1584,9 +1582,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:lumMod val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1639,7 +1635,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent5"/>
+              <a:srgbClr val="A94D0F"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -2044,7 +2040,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3"/>
+              <a:srgbClr val="FF5050"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -2097,9 +2093,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:lumMod val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -2152,7 +2146,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent5"/>
+              <a:srgbClr val="A94D0F"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -3018,7 +3012,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent6"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -3071,7 +3065,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3"/>
+              <a:srgbClr val="FF5050"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -3124,7 +3118,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent4"/>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -3177,7 +3171,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent5"/>
+              <a:srgbClr val="A94D0F"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -3230,7 +3224,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent6"/>
+              <a:srgbClr val="9E5ECE"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -3529,7 +3523,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent6"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -3582,7 +3576,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3"/>
+              <a:srgbClr val="FF5050"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -3635,7 +3629,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent4"/>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -3688,7 +3682,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent5"/>
+              <a:srgbClr val="A94D0F"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -3741,7 +3735,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent6"/>
+              <a:srgbClr val="9E5ECE"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -4040,7 +4034,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent6"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -4093,7 +4087,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3"/>
+              <a:srgbClr val="FF5050"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -4146,7 +4140,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent4"/>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -4199,7 +4193,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent5"/>
+              <a:srgbClr val="A94D0F"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -4252,7 +4246,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent6"/>
+              <a:srgbClr val="9E5ECE"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -4551,7 +4545,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent6"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -4604,7 +4598,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3"/>
+              <a:srgbClr val="FF5050"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -4657,7 +4651,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent4"/>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -4710,7 +4704,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent5"/>
+              <a:srgbClr val="A94D0F"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -4763,7 +4757,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent6"/>
+              <a:srgbClr val="9E5ECE"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -5583,9 +5577,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -6056,9 +6048,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:lumMod val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -6111,7 +6101,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent5"/>
+              <a:srgbClr val="A94D0F"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -6164,7 +6154,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent6"/>
+              <a:srgbClr val="9E5ECE"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -6516,7 +6506,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3"/>
+              <a:srgbClr val="FF5050"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -6569,9 +6559,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:lumMod val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -6624,7 +6612,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent5"/>
+              <a:srgbClr val="A94D0F"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -14988,9 +14976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA995AA-039D-463B-8703-8B0153A8BD40}">
   <dimension ref="A1:R95"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17241,7 +17227,7 @@
   <dimension ref="A1:R95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P60" sqref="P60"/>
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19681,12 +19667,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
     <mergeCell ref="O13:P13"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="B9:F9"/>
@@ -19694,6 +19674,12 @@
     <mergeCell ref="F13:H13"/>
     <mergeCell ref="I13:K13"/>
     <mergeCell ref="L13:N13"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>